<commit_message>
update ulva and benthic photoquadrat protocols
</commit_message>
<xml_diff>
--- a/benthic-photoquadrats/final_spreadsheets/benthic_photoquadrats_data_entry_spreadsheet_marinegeo.xlsx
+++ b/benthic-photoquadrats/final_spreadsheets/benthic_photoquadrats_data_entry_spreadsheet_marinegeo.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\benthic-photoquadrats\final_spreadsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957B7E5C-7990-4D1E-BF60-16BBA5999930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="glossary" sheetId="2" state="visible" r:id="rId1"/>
-    <sheet name="sample metadata" sheetId="3" state="visible" r:id="rId2"/>
+    <sheet name="glossary" sheetId="2" r:id="rId1"/>
+    <sheet name="sample metadata" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>definition</t>
   </si>
@@ -51,9 +58,6 @@
     </r>
   </si>
   <si>
-    <t>PROTOCOL NAME</t>
-  </si>
-  <si>
     <t>sheet name</t>
   </si>
   <si>
@@ -66,102 +70,101 @@
     <t>field name</t>
   </si>
   <si>
-    <t xml:space="preserve">BENTHIC PHOTOQUADRATS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOI: 10.25573/serc.14717823.v1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name(s) of data collector(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the specific location where the sample was collected; e.g., Curlew Cay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meter_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The meter along the transect at which the photo was taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numeric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photo_filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The filename of the image associated with the sample with the file extension included (e.g., "usa-mda_site1_t1_q1-unknown-seagrass.jpg")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photoquadrat_metadata_notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any additional notes regarding observations, context, or concerns about the data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_collection_day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The day the sample was collected in the field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_collection_month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The month the sample was collected in the field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_collection_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The year the sample was collected in the field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YYYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter your 6 character site code. Codes can be found in the standards section of the MarineGEO protocol website: https://marinegeo.github.io/standards/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX-YYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The transect at the location the sample came from: 1, 2, or 3</t>
+    <t>BENTHIC PHOTOQUADRATS</t>
+  </si>
+  <si>
+    <t>DOI: 10.25573/serc.14717823.v1</t>
+  </si>
+  <si>
+    <t>data_collector</t>
+  </si>
+  <si>
+    <t>Name(s) of data collector(s)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>sample metadata</t>
+  </si>
+  <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>The name of the specific location where the sample was collected; e.g., Curlew Cay</t>
+  </si>
+  <si>
+    <t>meter_number</t>
+  </si>
+  <si>
+    <t>The meter along the transect at which the photo was taken</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>photo_filename</t>
+  </si>
+  <si>
+    <t>The filename of the image associated with the sample with the file extension included (e.g., "usa-mda_site1_t1_q1-unknown-seagrass.jpg")</t>
+  </si>
+  <si>
+    <t>photoquadrat_metadata_notes</t>
+  </si>
+  <si>
+    <t>Any additional notes regarding observations, context, or concerns about the data.</t>
+  </si>
+  <si>
+    <t>sample_collection_day</t>
+  </si>
+  <si>
+    <t>The day the sample was collected in the field</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>sample_collection_month</t>
+  </si>
+  <si>
+    <t>The month the sample was collected in the field</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>sample_collection_year</t>
+  </si>
+  <si>
+    <t>The year the sample was collected in the field</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>site_code</t>
+  </si>
+  <si>
+    <t>Enter your 6 character site code. Codes can be found in the standards section of the MarineGEO protocol website: https://marinegeo.github.io/standards/</t>
+  </si>
+  <si>
+    <t>XXX-YYY</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>The transect at the location the sample came from: 1, 2, or 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,12 +173,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -185,20 +188,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <b/>
     </font>
     <font>
+      <b/>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <b/>
     </font>
     <font>
       <sz val="14"/>
@@ -208,10 +211,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -219,10 +222,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -271,11 +282,16 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -290,27 +306,39 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -323,18 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,6 +372,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -368,7 +385,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -713,248 +730,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="22" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46.5" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" ht="120" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" ht="32.25" customHeight="1">
+    <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="10" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -973,65 +990,67 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="22.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="12.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="14.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="27.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>23</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update data entry spreadsheet scripts
</commit_message>
<xml_diff>
--- a/benthic-photoquadrats/final_spreadsheets/benthic_photoquadrats_data_entry_spreadsheet_marinegeo.xlsx
+++ b/benthic-photoquadrats/final_spreadsheets/benthic_photoquadrats_data_entry_spreadsheet_marinegeo.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\benthic-photoquadrats\final_spreadsheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957B7E5C-7990-4D1E-BF60-16BBA5999930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="glossary" sheetId="2" r:id="rId1"/>
-    <sheet name="sample metadata" sheetId="3" r:id="rId2"/>
+    <sheet name="glossary" sheetId="2" state="visible" r:id="rId1"/>
+    <sheet name="sample metadata" sheetId="3" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>definition</t>
   </si>
@@ -58,6 +51,9 @@
     </r>
   </si>
   <si>
+    <t>PROTOCOL NAME</t>
+  </si>
+  <si>
     <t>sheet name</t>
   </si>
   <si>
@@ -70,101 +66,102 @@
     <t>field name</t>
   </si>
   <si>
-    <t>BENTHIC PHOTOQUADRATS</t>
-  </si>
-  <si>
-    <t>DOI: 10.25573/serc.14717823.v1</t>
-  </si>
-  <si>
-    <t>data_collector</t>
-  </si>
-  <si>
-    <t>Name(s) of data collector(s)</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>sample metadata</t>
-  </si>
-  <si>
-    <t>location_name</t>
-  </si>
-  <si>
-    <t>The name of the specific location where the sample was collected; e.g., Curlew Cay</t>
-  </si>
-  <si>
-    <t>meter_number</t>
-  </si>
-  <si>
-    <t>The meter along the transect at which the photo was taken</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>photo_filename</t>
-  </si>
-  <si>
-    <t>The filename of the image associated with the sample with the file extension included (e.g., "usa-mda_site1_t1_q1-unknown-seagrass.jpg")</t>
-  </si>
-  <si>
-    <t>photoquadrat_metadata_notes</t>
-  </si>
-  <si>
-    <t>Any additional notes regarding observations, context, or concerns about the data.</t>
-  </si>
-  <si>
-    <t>sample_collection_day</t>
-  </si>
-  <si>
-    <t>The day the sample was collected in the field</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>sample_collection_month</t>
-  </si>
-  <si>
-    <t>The month the sample was collected in the field</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>sample_collection_year</t>
-  </si>
-  <si>
-    <t>The year the sample was collected in the field</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>site_code</t>
-  </si>
-  <si>
-    <t>Enter your 6 character site code. Codes can be found in the standards section of the MarineGEO protocol website: https://marinegeo.github.io/standards/</t>
-  </si>
-  <si>
-    <t>XXX-YYY</t>
-  </si>
-  <si>
-    <t>transect</t>
-  </si>
-  <si>
-    <t>The transect at the location the sample came from: 1, 2, or 3</t>
+    <t xml:space="preserve">BENTHIC PHOTOQUADRATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOI: 10.25573/serc.14717823.v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name(s) of data collector(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the specific location where the sample was collected; e.g., Curlew Cay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meter_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The meter along the transect at which the photo was taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photo_filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The filename of the image associated with the sample with the file extension included (e.g., "usa-mda_site1_t1_q1-unknown-seagrass.jpg")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photoquadrat_metadata_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any additional notes regarding observations, context, or concerns about the data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_collection_day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The day the sample was collected in the field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_collection_month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The month the sample was collected in the field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_collection_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The year the sample was collected in the field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter your 6 character site code. Codes can be found in the standards section of the MarineGEO protocol website: https://marinegeo.github.io/standards/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX-YYY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The transect at the location the sample came from: 1, 2, or 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,12 +170,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -188,20 +185,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <b/>
     </font>
     <font>
       <sz val="14"/>
@@ -211,10 +208,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -222,18 +219,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -282,16 +271,11 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -306,39 +290,27 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -351,6 +323,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,7 +356,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,7 +368,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -730,248 +713,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="22" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" ht="46.5" customHeight="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="120" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -990,67 +973,65 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="22.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="12.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="14.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="27.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>22</v>
+    <row r="1">
+      <c r="A1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>